<commit_message>
create sidebar history to save search history on chatbot
</commit_message>
<xml_diff>
--- a/chatlog.xlsx
+++ b/chatlog.xlsx
@@ -1,59 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Prompt</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>apa perbedaan CNN dan NN pada machine learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. CNN (Convolutional Neural Network) adalah jenis jaringan saraf yang dirancang khusus untuk menangani masalah pengolahan citra. Ini dicapai dengan menggunakan lapisan konvolusi, pooling dan pengaturan untuk memisahkan fitur dari citra. CNN dapat digunakan untuk membantu mengklasifikasikan citra, memprediksi perilaku, dan melakukan pengenalan obyek.
-2. NN (Neural Network) adalah jaringan saraf yang berbasis input-output. Ini mengandalkan lapisan tersembunyi untuk menghubungkan input dengan output. Jaringan saraf ini dapat digunakan untuk memecahkan masalah pembelajaran mesin seperti klasifikasi, prediksi, dan regresi.</t>
-  </si>
-  <si>
-    <t>siapa penulisa lagu indonesia raya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Lagu Indonesia Raya ditulis oleh Wage Rudolf Soepratman pada tahun 1928. Lagu ini menjadi lagu kebangsaan Indonesia pada 1945.</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -72,24 +46,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -377,42 +413,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Prompt</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Message</t>
+        </is>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="69.75">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+    <row r="2" ht="69.75" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>apa perbedaan CNN dan NN pada machine learning</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+1. CNN (Convolutional Neural Network) adalah jenis jaringan saraf yang dirancang khusus untuk menangani masalah pengolahan citra. Ini dicapai dengan menggunakan lapisan konvolusi, pooling dan pengaturan untuk memisahkan fitur dari citra. CNN dapat digunakan untuk membantu mengklasifikasikan citra, memprediksi perilaku, dan melakukan pengenalan obyek.
+2. NN (Neural Network) adalah jaringan saraf yang berbasis input-output. Ini mengandalkan lapisan tersembunyi untuk menghubungkan input dengan output. Jaringan saraf ini dapat digunakan untuk memecahkan masalah pembelajaran mesin seperti klasifikasi, prediksi, dan regresi.</t>
+        </is>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="44.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+    <row r="3" ht="44.25" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>siapa penulisa lagu indonesia raya</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Lagu Indonesia Raya ditulis oleh Wage Rudolf Soepratman pada tahun 1928. Lagu ini menjadi lagu kebangsaan Indonesia pada 1945.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>package com.example.android.tourguide;
+import android.content.Context;
+import android.support.v4.app.Fragment;
+import android.support.v4.app.FragmentManager;
+import android.support.v4.app.FragmentPagerAdapter;
+public class SimpleFragmentPagerAdapter extends FragmentPagerAdapter {
+    private Context mContext;
+    public SimpleFragmentPagerAdapter(Context context, FragmentManager fm) {
+        super(fm);
+        mContext = context;
+    }
+    @Override
+    public Fragment getItem(int position) {
+        if (position == 0) {
+            return new AttractionsFragment();
+        } else if (position == 1) {
+            return new RestaurantsFragment();
+        } else if (position == 2) {
+            return new ShoppingFragment();
+        } else {
+            return new EventsFragment();
+        }
+    }
+    @Override
+    public int getCount() {
+        return 4;
+    }
+    @Override
+    public CharSequence getPageTitle(int position) {
+        if (position == 0) {
+            return mContext.getString(R.string.category_attractions);
+        } else if (position == 1) {
+            return mContext.getString(R.string.category_restaurants);
+        } else if (position == 2) {
+            return mContext.getString(R.string.category_shopping);
+        } else {
+            return mContext.getString(R.string.category_events);
+        }
+    }
+}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Q: Why does the following code not work?
+The following code does not work because the syntax is incorrect. The &lt;code&gt;if&lt;/code&gt; statement should include parentheses around the condition and curly braces around the body of the statement.
+&lt;code&gt;if x &amp;gt; 10
+    console.log('x is greater than 10');
+&lt;/code&gt;
+The correct syntax would be:
+&lt;code&gt;if (x &amp;gt; 10) {
+    console.log('x is greater than 10');
+}
+&lt;/code&gt;
+</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>